<commit_message>
new data file for Nemegt for TNN
</commit_message>
<xml_diff>
--- a/AIC_All Areas X combined.xlsx
+++ b/AIC_All Areas X combined.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koustubh\Dropbox (Snow Leopard Trust)\CREEM\Analyses\snowleopards\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="960" yWindow="915" windowWidth="19395" windowHeight="7155"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -159,7 +164,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -706,6 +711,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -753,7 +761,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -788,7 +796,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1000,9 +1008,10 @@
   <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" activePane="bottomLeft"/>
-      <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane xSplit="1350" ySplit="600" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,36 +1093,36 @@
         <v>2481.75</v>
       </c>
       <c r="L2" s="1">
-        <v>16.51014</v>
+        <v>14.2</v>
       </c>
       <c r="M2">
-        <v>1.963876</v>
+        <v>0.46</v>
       </c>
       <c r="N2">
-        <v>14.647857</v>
+        <v>14.01</v>
       </c>
       <c r="O2">
-        <v>23.725650000000002</v>
+        <v>16.88</v>
       </c>
       <c r="P2" s="2">
         <f>(L2-L6)/L6</f>
-        <v>0.15665744944833296</v>
+        <v>-0.10410094637223977</v>
       </c>
       <c r="Q2">
         <f>L2*100/K2</f>
-        <v>0.66526201269265639</v>
+        <v>0.5721768913065377</v>
       </c>
       <c r="R2">
         <f>M2*100/K2</f>
-        <v>7.913270877405057E-2</v>
+        <v>1.8535307746549812E-2</v>
       </c>
       <c r="S2">
         <f>N2*100/K2</f>
-        <v>0.59022290722272586</v>
+        <v>0.56452100332426713</v>
       </c>
       <c r="T2">
         <f>O2*100/K2</f>
-        <v>0.95600483529767299</v>
+        <v>0.6801652060038279</v>
       </c>
       <c r="V2">
         <v>17.600000000000001</v>
@@ -1142,33 +1151,33 @@
         <v>2481.75</v>
       </c>
       <c r="L6" s="1">
-        <v>14.274010000000001</v>
+        <v>15.85</v>
       </c>
       <c r="M6">
-        <v>0.54757540000000005</v>
+        <v>1.7</v>
       </c>
       <c r="N6">
-        <v>14.022821</v>
+        <v>14.39</v>
       </c>
       <c r="O6">
-        <v>17.28999</v>
+        <v>22.59</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6">
         <f>L6*100/K6</f>
-        <v>0.5751590611463685</v>
+        <v>0.63866223431046643</v>
       </c>
       <c r="R6">
         <f>M6*100/K6</f>
-        <v>2.2064083811826334E-2</v>
+        <v>6.8500050367684098E-2</v>
       </c>
       <c r="S6">
         <f>N6*100/K6</f>
-        <v>0.56503761458648138</v>
+        <v>0.57983277928880828</v>
       </c>
       <c r="T6">
         <f>O6*100/K6</f>
-        <v>0.69668540344514962</v>
+        <v>0.91024478694469624</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1229,7 +1238,7 @@
         <v>2145.5</v>
       </c>
       <c r="L14" s="1">
-        <v>23.75</v>
+        <v>20</v>
       </c>
       <c r="M14">
         <v>6.34</v>
@@ -1242,11 +1251,11 @@
       </c>
       <c r="P14" s="2">
         <f>(L14-L16)/L16</f>
-        <v>0.28239740820734344</v>
+        <v>8.0497028633171167E-2</v>
       </c>
       <c r="Q14">
         <f>L14*100/K14</f>
-        <v>1.1069680727103239</v>
+        <v>0.93218364017711486</v>
       </c>
       <c r="R14">
         <f>M14*100/K14</f>
@@ -1288,7 +1297,7 @@
         <v>2145.5</v>
       </c>
       <c r="L16" s="1">
-        <v>18.52</v>
+        <v>18.510000000000002</v>
       </c>
       <c r="M16">
         <v>2.48</v>
@@ -1302,7 +1311,7 @@
       <c r="P16" s="2"/>
       <c r="Q16">
         <f>L16*100/K16</f>
-        <v>0.86320205080400836</v>
+        <v>0.86273595898391997</v>
       </c>
       <c r="R16">
         <f>M16*100/K16</f>
@@ -1451,36 +1460,36 @@
         <v>2116.5</v>
       </c>
       <c r="L26" s="1">
-        <v>28.744720000000001</v>
+        <v>14.584</v>
       </c>
       <c r="M26">
-        <v>5.766534</v>
+        <v>0.83</v>
       </c>
       <c r="N26">
-        <v>23.107099999999999</v>
+        <v>14.07</v>
       </c>
       <c r="O26">
-        <v>49.465910000000001</v>
+        <v>18.59</v>
       </c>
       <c r="P26" s="2">
         <f>(L26-L31)/L31</f>
-        <v>0.10080390679092906</v>
+        <v>-7.0490758444869336E-2</v>
       </c>
       <c r="Q26">
         <f>L26*100/K26</f>
-        <v>1.3581252067091898</v>
+        <v>0.68906213087644685</v>
       </c>
       <c r="R26">
         <f>M26*100/K26</f>
-        <v>0.27245613040396882</v>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="S26">
         <f>N26*100/K26</f>
-        <v>1.091759981100874</v>
+        <v>0.66477675407512404</v>
       </c>
       <c r="T26">
         <f>O26*100/K26</f>
-        <v>2.3371561540278765</v>
+        <v>0.87833687691944251</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -1508,32 +1517,32 @@
         <v>2116.5</v>
       </c>
       <c r="L31" s="1">
-        <v>26.112480000000001</v>
+        <v>15.69</v>
       </c>
       <c r="M31">
-        <v>2.7644669999999998</v>
+        <v>1.62</v>
       </c>
       <c r="N31">
-        <v>22.8947</v>
+        <v>14.34</v>
       </c>
       <c r="O31">
-        <v>34.795029999999997</v>
+        <v>22.22</v>
       </c>
       <c r="Q31">
         <f>L31*100/K31</f>
-        <v>1.2337576187101347</v>
+        <v>0.74131821403260101</v>
       </c>
       <c r="R31">
         <f>M31*100/K31</f>
-        <v>0.13061502480510276</v>
+        <v>7.6541459957476965E-2</v>
       </c>
       <c r="S31">
         <f>N31*100/K31</f>
-        <v>1.0817245452397828</v>
+        <v>0.67753366406803683</v>
       </c>
       <c r="T31">
         <f>O31*100/K31</f>
-        <v>1.6439891330025984</v>
+        <v>1.0498464446019371</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>